<commit_message>
updated analyses and tidied up the code
</commit_message>
<xml_diff>
--- a/__contacted_authors.xlsx
+++ b/__contacted_authors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jottacloud\PDtremor_syst-review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8EE396-780F-4FDA-A825-9FDE8E23131E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF1C80F-B3C9-4374-BB64-7AA4A0FCE8CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16386" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="97">
   <si>
     <t>Contacted authors</t>
   </si>
@@ -295,9 +294,6 @@
     <t>TEVA unwilling to provide data</t>
   </si>
   <si>
-    <t>Zambon unwilling to provide data</t>
-  </si>
-  <si>
     <t>received data</t>
   </si>
   <si>
@@ -308,6 +304,18 @@
   </si>
   <si>
     <t>author not responsible for data</t>
+  </si>
+  <si>
+    <t>Data was provided</t>
+  </si>
+  <si>
+    <t>Data was not provided</t>
+  </si>
+  <si>
+    <t>Data was available elsewhere</t>
+  </si>
+  <si>
+    <t>data was included in other study according to author</t>
   </si>
 </sst>
 </file>
@@ -747,14 +755,14 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="37.15625" customWidth="1"/>
     <col min="2" max="2" width="47.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.9453125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.05078125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
   </cols>
@@ -850,7 +858,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="4">
         <v>44386</v>
@@ -870,6 +878,9 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
       <c r="D6" s="4">
         <v>44386</v>
       </c>
@@ -888,6 +899,9 @@
       <c r="B7" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
       <c r="D7" s="4">
         <v>44387</v>
       </c>
@@ -908,6 +922,9 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
       <c r="D8" s="4">
         <v>44388</v>
       </c>
@@ -948,7 +965,7 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -966,6 +983,9 @@
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" t="s">
@@ -982,6 +1002,9 @@
       <c r="B12" t="s">
         <v>30</v>
       </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" t="s">
@@ -1036,6 +1059,9 @@
       <c r="B15" t="s">
         <v>39</v>
       </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" t="s">
@@ -1050,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1087,6 +1113,9 @@
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" t="s">
@@ -1103,6 +1132,9 @@
       <c r="B19" t="s">
         <v>50</v>
       </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
       <c r="D19" s="4">
         <v>44441</v>
       </c>
@@ -1165,6 +1197,9 @@
       <c r="B22" t="s">
         <v>58</v>
       </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
       <c r="D22" s="4">
         <v>44472</v>
       </c>
@@ -1184,7 +1219,7 @@
         <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="4">
         <v>44475</v>
@@ -1204,6 +1239,9 @@
       <c r="B24" t="s">
         <v>62</v>
       </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
       <c r="D24" s="4">
         <v>44475</v>
       </c>
@@ -1245,6 +1283,9 @@
       <c r="B26" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
       <c r="D26" s="4">
         <v>44508</v>
       </c>
@@ -1258,7 +1299,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
@@ -1281,6 +1322,9 @@
       <c r="B28" t="s">
         <v>70</v>
       </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
       <c r="D28" s="4">
         <v>44511</v>
       </c>
@@ -1299,6 +1343,9 @@
       <c r="B29" t="s">
         <v>73</v>
       </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
       <c r="D29" s="4">
         <v>44514</v>
       </c>
@@ -1377,6 +1424,9 @@
       <c r="B33" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
       <c r="D33" s="4">
         <v>44583</v>
       </c>
@@ -1395,6 +1445,9 @@
       <c r="B34" t="s">
         <v>83</v>
       </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
       <c r="D34" s="4">
         <v>44583</v>
       </c>
@@ -1413,6 +1466,9 @@
       <c r="B35" t="s">
         <v>84</v>
       </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
       <c r="D35" s="4">
         <v>44587</v>
       </c>
@@ -1421,7 +1477,7 @@
         <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>